<commit_message>
Add Exception useCase Mot de pqsse incorrect et qcces refuse Amplitude
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talents\Documents\UiPath\RobTalent_UpdateChapter_Amplitude_TALENT_v1.0\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim Gueye\Documents\UiPath\RobTalent_UpdateChapter_Amplitude_TALENT_v1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34609B0-6FFA-4CC0-A88B-C68E87010079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9D7CF-B056-49EA-B976-493F9AF5A784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -207,13 +207,13 @@
     <t>MaxRetryCapture</t>
   </si>
   <si>
-    <t>ROBTALENTS</t>
-  </si>
-  <si>
     <t>C:\Users\Talents\Documents\UiPath\RobTalent_UpdateChapter_Amplitude_TALENT_v1.0\Data\Output\</t>
   </si>
   <si>
     <t>talent</t>
+  </si>
+  <si>
+    <t>IBATEST</t>
   </si>
 </sst>
 </file>
@@ -623,15 +623,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="90.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="90.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -679,7 +679,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -689,7 +689,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -705,7 +705,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -737,7 +737,7 @@
         <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -745,7 +745,7 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -1760,12 +1760,12 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1802,7 +1802,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1927,7 +1927,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2961,12 +2961,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>